<commit_message>
Date10th may 2016 update report
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -1508,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="H54" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1521,7 @@
     <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
@@ -5315,7 +5315,7 @@
     <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="255" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="21.28515625" style="8" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Reports of 11th May
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -1508,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView topLeftCell="H6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -1521,7 +1521,7 @@
     <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
@@ -5315,7 +5315,7 @@
     <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="21.28515625" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="255" style="8" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Reports commited of 12th May 2016
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -1508,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="H6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -1521,7 +1521,7 @@
     <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
@@ -5299,7 +5299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
@@ -5315,7 +5315,7 @@
     <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="255" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="21.28515625" style="8" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Reports commited for 13th May 2016
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="273">
   <si>
     <t>TCID</t>
   </si>
@@ -834,9 +834,6 @@
   </si>
   <si>
     <t>campaign_button</t>
-  </si>
-  <si>
-    <t>ExplicitWait</t>
   </si>
   <si>
     <t>TS075</t>
@@ -1463,11 +1460,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
+    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1508,23 +1505,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" style="2" collapsed="1"/>
-    <col min="3" max="3" width="31.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="31.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="32.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
+    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -2267,11 +2271,9 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>89</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E16" s="11"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" t="s">
@@ -5181,7 +5183,7 @@
         <v>32</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>200</v>
@@ -5230,7 +5232,7 @@
         <v>32</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>235</v>
@@ -5305,18 +5307,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="21.28515625" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
+    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
+    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="6.3984375" collapsed="true"/>
+    <col min="24" max="16384" style="8" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Report commited for 16th May 2016
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="273">
   <si>
     <t>TCID</t>
   </si>
@@ -1460,11 +1460,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
-    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,30 +1505,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="H6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="31.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="32.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
-    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="11" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" style="2" collapsed="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5301,24 +5294,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
-    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
-    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
-    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="6.3984375" collapsed="true"/>
-    <col min="24" max="16384" style="8" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="255" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Report commited for 17th May 2016
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="273">
   <si>
     <t>TCID</t>
   </si>
@@ -1460,11 +1460,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
+    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,17 +1511,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" style="2" collapsed="1"/>
-    <col min="3" max="3" width="31.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="31.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="32.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
+    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5300,18 +5307,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="255" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
+    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
+    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="6.3984375" collapsed="true"/>
+    <col min="24" max="16384" style="8" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reports commited for 18th May 2016
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="273">
   <si>
     <t>TCID</t>
   </si>
@@ -1460,11 +1460,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
-    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,30 +1505,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="H6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="H6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="31.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="32.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
-    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="11" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" style="2" collapsed="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5301,24 +5294,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
-    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
-    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
-    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="6.3984375" collapsed="true"/>
-    <col min="24" max="16384" style="8" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="255" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Report commited for 19th May 2016 and 2 fix made in locators
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="273">
   <si>
     <t>TCID</t>
   </si>
@@ -1460,11 +1460,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
+    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,17 +1511,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" style="2" collapsed="1"/>
-    <col min="3" max="3" width="31.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="31.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="32.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
+    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5300,18 +5307,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="255" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
+    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
+    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="6.3984375" collapsed="true"/>
+    <col min="24" max="16384" style="8" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reports commited for 23 May 16
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2909" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="273">
   <si>
     <t>TCID</t>
   </si>
@@ -1460,11 +1460,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
-    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,30 +1505,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H6" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="G7" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="31.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="32.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
-    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="11" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" style="2" collapsed="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5301,24 +5294,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
-    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
-    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
-    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="6.3984375" collapsed="true"/>
-    <col min="24" max="16384" style="8" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="255" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reports committed and increased the implicit wait from 20 seconds to 2 minuts
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="273">
   <si>
     <t>TCID</t>
   </si>
@@ -1460,11 +1460,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
+    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,17 +1511,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" style="2" collapsed="1"/>
-    <col min="3" max="3" width="31.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="31.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="32.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
+    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5298,18 +5305,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="255" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
+    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
+    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="6.3984375" collapsed="true"/>
+    <col min="24" max="16384" style="8" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reports commited for 30th May 2016
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4449" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="273">
   <si>
     <t>TCID</t>
   </si>
@@ -1454,17 +1454,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
-    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,30 +1505,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="G7" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="E7" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="31.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="32.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
-    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="11" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" style="2" collapsed="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5301,22 +5294,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
-    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
-    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
-    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="6.3984375" collapsed="true"/>
-    <col min="24" max="16384" style="8" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="62" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reports committed for 01st June
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="273">
   <si>
     <t>TCID</t>
   </si>
@@ -1455,16 +1455,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
+    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,17 +1511,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" style="2" collapsed="1"/>
-    <col min="3" max="3" width="31.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="31.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="32.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
+    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5300,18 +5307,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="62" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="16384" width="8.85546875" style="8" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
+    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
+    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="6.3984375" collapsed="true"/>
+    <col min="24" max="16384" style="8" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reports commited for 3rd June
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -1454,7 +1454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1505,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5301,9 +5301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Reports commited and latest code push for backstage test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11415" windowHeight="2820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="297">
   <si>
     <t>TCID</t>
   </si>
@@ -840,6 +840,78 @@
   </si>
   <si>
     <t>TS076</t>
+  </si>
+  <si>
+    <t>Click on Wrench icon of created Campaign</t>
+  </si>
+  <si>
+    <t>clickWrenchOnCurrentCampaign</t>
+  </si>
+  <si>
+    <t>TS077</t>
+  </si>
+  <si>
+    <t>TS078</t>
+  </si>
+  <si>
+    <t>TS079</t>
+  </si>
+  <si>
+    <t>Click On Submit button</t>
+  </si>
+  <si>
+    <t>Set New Offer Status</t>
+  </si>
+  <si>
+    <t>set_offerStatus</t>
+  </si>
+  <si>
+    <t>Offer_status</t>
+  </si>
+  <si>
+    <t>Published</t>
+  </si>
+  <si>
+    <t>Outreach_status</t>
+  </si>
+  <si>
+    <t>set_outreachStatus</t>
+  </si>
+  <si>
+    <t>TS080</t>
+  </si>
+  <si>
+    <t>TS081</t>
+  </si>
+  <si>
+    <t>Set New Outreach Status</t>
+  </si>
+  <si>
+    <t>col|Offer_status</t>
+  </si>
+  <si>
+    <t>col|Outreach_status</t>
+  </si>
+  <si>
+    <t>submit_campaign</t>
+  </si>
+  <si>
+    <t>Set Video Due date</t>
+  </si>
+  <si>
+    <t>campaignDueDate</t>
+  </si>
+  <si>
+    <t>TS082</t>
+  </si>
+  <si>
+    <t>TS083</t>
+  </si>
+  <si>
+    <t>TS084</t>
+  </si>
+  <si>
+    <t>TS085</t>
   </si>
 </sst>
 </file>
@@ -1460,11 +1532,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
-    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1503,32 +1575,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView topLeftCell="A62" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="31.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="32.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
-    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="9.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5235,10 +5299,10 @@
         <v>272</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>19</v>
+        <v>274</v>
       </c>
       <c r="E77" s="11"/>
       <c r="F77" s="4"/>
@@ -5275,17 +5339,454 @@
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A78" s="28"/>
-      <c r="B78" s="29"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
-      <c r="G78" s="30"/>
+      <c r="A78" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="G78" s="4"/>
+      <c r="H78" t="s">
+        <v>20</v>
+      </c>
+      <c r="I78" t="s">
+        <v>21</v>
+      </c>
+      <c r="J78" t="s">
+        <v>21</v>
+      </c>
+      <c r="K78" t="s">
+        <v>21</v>
+      </c>
+      <c r="L78" t="s">
+        <v>21</v>
+      </c>
+      <c r="M78" t="s">
+        <v>21</v>
+      </c>
+      <c r="N78" t="s">
+        <v>21</v>
+      </c>
+      <c r="O78" t="s">
+        <v>21</v>
+      </c>
+      <c r="P78" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" t="s">
+        <v>20</v>
+      </c>
+      <c r="I79" t="s">
+        <v>21</v>
+      </c>
+      <c r="J79" t="s">
+        <v>21</v>
+      </c>
+      <c r="K79" t="s">
+        <v>21</v>
+      </c>
+      <c r="L79" t="s">
+        <v>21</v>
+      </c>
+      <c r="M79" t="s">
+        <v>21</v>
+      </c>
+      <c r="N79" t="s">
+        <v>21</v>
+      </c>
+      <c r="O79" t="s">
+        <v>21</v>
+      </c>
+      <c r="P79" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E80" s="11"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" t="s">
+        <v>20</v>
+      </c>
+      <c r="I80" t="s">
+        <v>21</v>
+      </c>
+      <c r="J80" t="s">
+        <v>21</v>
+      </c>
+      <c r="K80" t="s">
+        <v>21</v>
+      </c>
+      <c r="L80" t="s">
+        <v>21</v>
+      </c>
+      <c r="M80" t="s">
+        <v>21</v>
+      </c>
+      <c r="N80" t="s">
+        <v>21</v>
+      </c>
+      <c r="O80" t="s">
+        <v>21</v>
+      </c>
+      <c r="P80" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G81" s="4"/>
+      <c r="H81" t="s">
+        <v>20</v>
+      </c>
+      <c r="I81" t="s">
+        <v>21</v>
+      </c>
+      <c r="J81" t="s">
+        <v>21</v>
+      </c>
+      <c r="K81" t="s">
+        <v>21</v>
+      </c>
+      <c r="L81" t="s">
+        <v>21</v>
+      </c>
+      <c r="M81" t="s">
+        <v>21</v>
+      </c>
+      <c r="N81" t="s">
+        <v>21</v>
+      </c>
+      <c r="O81" t="s">
+        <v>21</v>
+      </c>
+      <c r="P81" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" t="s">
+        <v>20</v>
+      </c>
+      <c r="I82" t="s">
+        <v>21</v>
+      </c>
+      <c r="J82" t="s">
+        <v>21</v>
+      </c>
+      <c r="K82" t="s">
+        <v>21</v>
+      </c>
+      <c r="L82" t="s">
+        <v>21</v>
+      </c>
+      <c r="M82" t="s">
+        <v>21</v>
+      </c>
+      <c r="N82" t="s">
+        <v>21</v>
+      </c>
+      <c r="O82" t="s">
+        <v>21</v>
+      </c>
+      <c r="P82" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E83" s="11"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" t="s">
+        <v>20</v>
+      </c>
+      <c r="I83" t="s">
+        <v>21</v>
+      </c>
+      <c r="J83" t="s">
+        <v>21</v>
+      </c>
+      <c r="K83" t="s">
+        <v>21</v>
+      </c>
+      <c r="L83" t="s">
+        <v>21</v>
+      </c>
+      <c r="M83" t="s">
+        <v>21</v>
+      </c>
+      <c r="N83" t="s">
+        <v>21</v>
+      </c>
+      <c r="O83" t="s">
+        <v>21</v>
+      </c>
+      <c r="P83" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="E84" s="11"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" t="s">
+        <v>20</v>
+      </c>
+      <c r="I84" t="s">
+        <v>21</v>
+      </c>
+      <c r="J84" t="s">
+        <v>21</v>
+      </c>
+      <c r="K84" t="s">
+        <v>21</v>
+      </c>
+      <c r="L84" t="s">
+        <v>21</v>
+      </c>
+      <c r="M84" t="s">
+        <v>21</v>
+      </c>
+      <c r="N84" t="s">
+        <v>21</v>
+      </c>
+      <c r="O84" t="s">
+        <v>21</v>
+      </c>
+      <c r="P84" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" t="s">
+        <v>20</v>
+      </c>
+      <c r="I85" t="s">
+        <v>21</v>
+      </c>
+      <c r="J85" t="s">
+        <v>21</v>
+      </c>
+      <c r="K85" t="s">
+        <v>21</v>
+      </c>
+      <c r="L85" t="s">
+        <v>21</v>
+      </c>
+      <c r="M85" t="s">
+        <v>21</v>
+      </c>
+      <c r="N85" t="s">
+        <v>21</v>
+      </c>
+      <c r="O85" t="s">
+        <v>21</v>
+      </c>
+      <c r="P85" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E86" s="11"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" t="s">
+        <v>20</v>
+      </c>
+      <c r="I86" t="s">
+        <v>21</v>
+      </c>
+      <c r="J86" t="s">
+        <v>21</v>
+      </c>
+      <c r="K86" t="s">
+        <v>21</v>
+      </c>
+      <c r="L86" t="s">
+        <v>21</v>
+      </c>
+      <c r="M86" t="s">
+        <v>21</v>
+      </c>
+      <c r="N86" t="s">
+        <v>21</v>
+      </c>
+      <c r="O86" t="s">
+        <v>21</v>
+      </c>
+      <c r="P86" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" s="28"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A87:G87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -5299,27 +5800,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
-    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
-    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
-    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="8" width="6.3984375" collapsed="true"/>
-    <col min="24" max="16384" style="8" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="20" max="22" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.42578125" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="16384" width="8.85546875" style="8" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
@@ -5381,16 +5884,22 @@
         <v>13</v>
       </c>
       <c r="U1" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>103</v>
       </c>
@@ -5447,15 +5956,21 @@
         <v>259</v>
       </c>
       <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
+      <c r="U2" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="V2" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y2" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>103</v>
       </c>
@@ -5512,15 +6027,21 @@
         <v>259</v>
       </c>
       <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
+      <c r="U3" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="V3" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W3" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y3" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>103</v>
       </c>
@@ -5577,15 +6098,21 @@
         <v>259</v>
       </c>
       <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
+      <c r="U4" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="V4" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W4" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y4" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>103</v>
       </c>
@@ -5642,15 +6169,21 @@
         <v>259</v>
       </c>
       <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
+      <c r="U5" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="V5" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W5" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y5" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>103</v>
       </c>
@@ -5707,15 +6240,21 @@
         <v>259</v>
       </c>
       <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
+      <c r="U6" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="V6" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W6" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y6" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>103</v>
       </c>
@@ -5772,15 +6311,21 @@
         <v>259</v>
       </c>
       <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
+      <c r="U7" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="V7" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W7" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y7" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>103</v>
       </c>
@@ -5837,15 +6382,21 @@
         <v>259</v>
       </c>
       <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
+      <c r="U8" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="V8" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W8" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y8" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>103</v>
       </c>
@@ -5902,15 +6453,21 @@
         <v>259</v>
       </c>
       <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
+      <c r="U9" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="V9" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W9" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y9" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>103</v>
       </c>
@@ -5967,15 +6524,21 @@
         <v>259</v>
       </c>
       <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
+      <c r="U10" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="V10" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W10" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y10" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>103</v>
       </c>
@@ -6032,11 +6595,17 @@
         <v>259</v>
       </c>
       <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
+      <c r="U11" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="V11" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W11" s="10" t="s">
+      <c r="Y11" s="10" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
video & manage cases merge
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
+++ b/src/test/java/com/genvideo/xls/Backstage_Test_Cases.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Steps" sheetId="2" r:id="rId2"/>
     <sheet name="Generate" sheetId="3" r:id="rId3"/>
+    <sheet name="Manage" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Steps'!$A$1:$Q$86</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="360">
   <si>
     <t>TCID</t>
   </si>
@@ -929,13 +930,242 @@
     <t>Title</t>
   </si>
   <si>
-    <t>FAIL -- Not able to click on linkElement is not currently visible and so may not be interacted with
+    <t>Manage</t>
+  </si>
+  <si>
+    <t>Click on content button</t>
+  </si>
+  <si>
+    <t>content_link</t>
+  </si>
+  <si>
+    <t>video_thumbnail</t>
+  </si>
+  <si>
+    <t>full_video_info</t>
+  </si>
+  <si>
+    <t>Click on video thumbnail</t>
+  </si>
+  <si>
+    <t>Click on video full information</t>
+  </si>
+  <si>
+    <t>createVideoList</t>
+  </si>
+  <si>
+    <t>Create a list and add videos</t>
+  </si>
+  <si>
+    <t>Click on video title</t>
+  </si>
+  <si>
+    <t>backstageTestVideo</t>
+  </si>
+  <si>
+    <t>player_state1</t>
+  </si>
+  <si>
+    <t>Play</t>
+  </si>
+  <si>
+    <t>player_state2</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>Pause the video</t>
+  </si>
+  <si>
+    <t>Click on email link</t>
+  </si>
+  <si>
+    <t>manage_email</t>
+  </si>
+  <si>
+    <t>writeInInputID</t>
+  </si>
+  <si>
+    <t>email_friend</t>
+  </si>
+  <si>
+    <t>col|email_friend</t>
+  </si>
+  <si>
+    <t>genvideotest5@gmail.com</t>
+  </si>
+  <si>
+    <t>Type friend's email</t>
+  </si>
+  <si>
+    <t>Click on send button</t>
+  </si>
+  <si>
+    <t>email_send</t>
+  </si>
+  <si>
+    <t>Click on manage images</t>
+  </si>
+  <si>
+    <t>manage_images</t>
+  </si>
+  <si>
+    <t>manage_show_images</t>
+  </si>
+  <si>
+    <t>Click on show more images</t>
+  </si>
+  <si>
+    <t>manage_select_image</t>
+  </si>
+  <si>
+    <t>Mouse hover an image</t>
+  </si>
+  <si>
+    <t>mouseHover</t>
+  </si>
+  <si>
+    <t>Select the hovered image</t>
+  </si>
+  <si>
+    <t>manage_select_preview</t>
+  </si>
+  <si>
+    <t>Mouse hover to set as default</t>
+  </si>
+  <si>
+    <t>manage_image_default</t>
+  </si>
+  <si>
+    <t>manage_image_download</t>
+  </si>
+  <si>
+    <t>Close manage image</t>
+  </si>
+  <si>
+    <t>close_manage_image</t>
+  </si>
+  <si>
+    <t>manage_lists</t>
+  </si>
+  <si>
+    <t>Click on lists link</t>
+  </si>
+  <si>
+    <t>Wait for 25 sec to play video</t>
+  </si>
+  <si>
+    <t>Wait for page to load</t>
+  </si>
+  <si>
+    <t>Download the image file</t>
+  </si>
+  <si>
+    <t>downloadImage</t>
+  </si>
+  <si>
+    <t>Mouse hover on any image</t>
+  </si>
+  <si>
+    <t>config|browserType1</t>
+  </si>
+  <si>
+    <t>mouseHoverAndClick</t>
+  </si>
+  <si>
+    <t>Email the list created</t>
+  </si>
+  <si>
+    <t>emailList</t>
+  </si>
+  <si>
+    <t>FAIL -- text not verified  -- Wrong pixel ratio - images must be square</t>
+  </si>
+  <si>
+    <t>manageVideo_title</t>
+  </si>
+  <si>
+    <t>FAIL -- Not able to click on linkno such element: Unable to locate element: {"method":"xpath","selector":"(//div[contains(text(),'List20160808141513')]//ancestor::a//button[@type='button'])[2]"}
+  (Session info: chrome=51.0.2704.103)
+  (Driver info: chromedriver=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4),platform=Windows NT 6.1 SP1 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 20.05 seconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '2.53.0', revision: '35ae25b1534ae328c771e0856c93e187490ca824', time: '2016-03-15 10:43:46'
+System info: host: 'pclap-002', ip: '172.16.146.137', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, chrome={chromedriverVersion=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4), userDataDir=C:\Users\user\AppData\Local\Temp\scoped_dir3084_15681}, takesHeapSnapshot=true, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=51.0.2704.103, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
+Session ID: 6eadaa40394f8c002cdb871dc05d8d65
+*** Element info: {Using=xpath, value=(//div[contains(text(),'List20160808141513')]//ancestor::a//button[@type='button'])[2]}</t>
+  </si>
+  <si>
+    <t>FAIL -- Not able to click on linkno such element: Unable to locate element: {"method":"xpath","selector":"(//div[contains(text(),'List20160808142113')]//ancestor::a//button[@type='button'])[2]"}
+  (Session info: chrome=51.0.2704.103)
+  (Driver info: chromedriver=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4),platform=Windows NT 6.1 SP1 x86_64) (WARNING: The server did not provide any stacktrace information)
 Command duration or timeout: 20.04 seconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
 Build info: version: '2.53.0', revision: '35ae25b1534ae328c771e0856c93e187490ca824', time: '2016-03-15 10:43:46'
-System info: host: 'pclap-002', ip: '172.16.146.187', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=46.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=false, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 6e154371-3511-427f-91c6-310f3b9e1f89</t>
+System info: host: 'pclap-002', ip: '172.16.146.137', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, chrome={chromedriverVersion=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4), userDataDir=C:\Users\user\AppData\Local\Temp\scoped_dir7332_13078}, takesHeapSnapshot=true, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=51.0.2704.103, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
+Session ID: c6145e0f679c466751f955d651885fbc
+*** Element info: {Using=xpath, value=(//div[contains(text(),'List20160808142113')]//ancestor::a//button[@type='button'])[2]}</t>
+  </si>
+  <si>
+    <t>FAIL -- Not able to click on linkTimed out after 90 seconds waiting for presence of element located by: By.xpath: //div[@class='spinner-container short ng-hide']
+Build info: version: '2.53.0', revision: '35ae25b1534ae328c771e0856c93e187490ca824', time: '2016-03-15 10:43:46'
+System info: host: 'pclap-002', ip: '172.16.146.137', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, chrome={chromedriverVersion=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4), userDataDir=C:\Users\user\AppData\Local\Temp\scoped_dir7632_28126}, takesHeapSnapshot=true, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=51.0.2704.103, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
+Session ID: 124c02b48a6f657123d724ee9c57ccd1</t>
+  </si>
+  <si>
+    <t>FAIL -- Not able to click on linkno such element: Unable to locate element: {"method":"xpath","selector":"email_send"}
+  (Session info: chrome=51.0.2704.103)
+  (Driver info: chromedriver=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4),platform=Windows NT 6.1 SP1 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 20.07 seconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '2.53.0', revision: '35ae25b1534ae328c771e0856c93e187490ca824', time: '2016-03-15 10:43:46'
+System info: host: 'pclap-002', ip: '172.16.146.137', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, chrome={chromedriverVersion=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4), userDataDir=C:\Users\user\AppData\Local\Temp\scoped_dir8100_24104}, takesHeapSnapshot=true, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=51.0.2704.103, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
+Session ID: 6c62407888d0cc8c5466753aa5e175ea
+*** Element info: {Using=xpath, value=email_send}</t>
+  </si>
+  <si>
+    <t>FAIL -- Not able to click on linkno such element: Unable to locate element: {"method":"xpath","selector":"email_send"}
+  (Session info: chrome=51.0.2704.103)
+  (Driver info: chromedriver=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4),platform=Windows NT 6.1 SP1 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 20.04 seconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '2.53.0', revision: '35ae25b1534ae328c771e0856c93e187490ca824', time: '2016-03-15 10:43:46'
+System info: host: 'pclap-002', ip: '172.16.146.137', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, chrome={chromedriverVersion=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4), userDataDir=C:\Users\user\AppData\Local\Temp\scoped_dir6104_12586}, takesHeapSnapshot=true, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=51.0.2704.103, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
+Session ID: 20fe9aa7803b99588cbd896b41812d57
+*** Element info: {Using=xpath, value=email_send}</t>
+  </si>
+  <si>
+    <t>FAIL Unable to write element not visible
+  (Session info: chrome=51.0.2704.103)
+  (Driver info: chromedriver=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4),platform=Windows NT 6.1 SP1 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 48 milliseconds
+Build info: version: '2.53.0', revision: '35ae25b1534ae328c771e0856c93e187490ca824', time: '2016-03-15 10:43:46'
+System info: host: 'pclap-002', ip: '172.16.146.137', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, chrome={chromedriverVersion=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4), userDataDir=C:\Users\user\AppData\Local\Temp\scoped_dir624_14359}, takesHeapSnapshot=true, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=51.0.2704.103, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
+Session ID: 73b7a4ce1755a84c29255cc06623d332</t>
+  </si>
+  <si>
+    <t>FAIL -- Not able to click on linkunknown error: Element is not clickable at point (203, 228). Other element would receive the click: &lt;div class="modal ng-scope top am-fade" id="myModal" role="dialog" aria-labelledby="myModalLabel" aria-hidden="true" tabindex="-1" style="z-index: 1050; display: block;"&gt;...&lt;/div&gt;
+  (Session info: chrome=51.0.2704.103)
+  (Driver info: chromedriver=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4),platform=Windows NT 6.1 SP1 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 78 milliseconds
+Build info: version: '2.53.0', revision: '35ae25b1534ae328c771e0856c93e187490ca824', time: '2016-03-15 10:43:46'
+System info: host: 'pclap-002', ip: '172.16.146.137', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, chrome={chromedriverVersion=2.21.371459 (36d3d07f660ff2bc1bf28a75d1cdabed0983e7c4), userDataDir=C:\Users\user\AppData\Local\Temp\scoped_dir624_14359}, takesHeapSnapshot=true, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=51.0.2704.103, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
+Session ID: 73b7a4ce1755a84c29255cc06623d332</t>
   </si>
 </sst>
 </file>
@@ -945,7 +1175,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1170,7 +1400,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1215,9 +1445,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1548,7 +1779,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1556,11 +1787,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="16.140625" collapsed="true"/>
+    <col min="5" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1583,9 +1814,19 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1599,22 +1840,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q87"/>
+  <dimension ref="A1:Q119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="9.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="6.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="38.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="30.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="28.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="27.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="15.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="255.0" collapsed="true"/>
+    <col min="9" max="16" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.5703125" collapsed="true"/>
+    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5476,7 +5720,7 @@
       <c r="E80" s="11"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
-      <c r="H80" t="s">
+      <c r="H80" s="28" t="s">
         <v>20</v>
       </c>
       <c r="I80" t="s">
@@ -5798,20 +6042,856 @@
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A87" s="28"/>
-      <c r="B87" s="29"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="29"/>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
-      <c r="G87" s="30"/>
+      <c r="A87" s="29"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="30"/>
+      <c r="G87" s="31"/>
+      <c r="I87"/>
+      <c r="J87"/>
+      <c r="K87"/>
+      <c r="L87"/>
+      <c r="M87"/>
+      <c r="N87"/>
+      <c r="O87"/>
+      <c r="P87"/>
+      <c r="Q87"/>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="G88" s="4"/>
+      <c r="H88" t="s">
+        <v>20</v>
+      </c>
+      <c r="I88" t="s">
+        <v>21</v>
+      </c>
+      <c r="J88" t="s">
+        <v>21</v>
+      </c>
+      <c r="K88" t="s">
+        <v>21</v>
+      </c>
+      <c r="L88" t="s">
+        <v>21</v>
+      </c>
+      <c r="M88" t="s">
+        <v>21</v>
+      </c>
+      <c r="N88" t="s">
+        <v>21</v>
+      </c>
+      <c r="O88" t="s">
+        <v>21</v>
+      </c>
+      <c r="P88" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G89" s="4"/>
+      <c r="H89" t="s">
+        <v>20</v>
+      </c>
+      <c r="I89" t="s">
+        <v>21</v>
+      </c>
+      <c r="J89" t="s">
+        <v>21</v>
+      </c>
+      <c r="K89" t="s">
+        <v>21</v>
+      </c>
+      <c r="L89" t="s">
+        <v>21</v>
+      </c>
+      <c r="M89" t="s">
+        <v>21</v>
+      </c>
+      <c r="N89" t="s">
+        <v>21</v>
+      </c>
+      <c r="O89" t="s">
+        <v>21</v>
+      </c>
+      <c r="P89" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G90" s="4"/>
+      <c r="H90" t="s">
+        <v>20</v>
+      </c>
+      <c r="I90" t="s">
+        <v>21</v>
+      </c>
+      <c r="J90" t="s">
+        <v>21</v>
+      </c>
+      <c r="K90" t="s">
+        <v>21</v>
+      </c>
+      <c r="L90" t="s">
+        <v>21</v>
+      </c>
+      <c r="M90" t="s">
+        <v>21</v>
+      </c>
+      <c r="N90" t="s">
+        <v>21</v>
+      </c>
+      <c r="O90" t="s">
+        <v>21</v>
+      </c>
+      <c r="P90" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G91" s="4"/>
+      <c r="H91" t="s">
+        <v>20</v>
+      </c>
+      <c r="I91" t="s">
+        <v>21</v>
+      </c>
+      <c r="J91" t="s">
+        <v>21</v>
+      </c>
+      <c r="K91" t="s">
+        <v>21</v>
+      </c>
+      <c r="L91" t="s">
+        <v>21</v>
+      </c>
+      <c r="M91" t="s">
+        <v>21</v>
+      </c>
+      <c r="N91" t="s">
+        <v>21</v>
+      </c>
+      <c r="O91" t="s">
+        <v>21</v>
+      </c>
+      <c r="P91" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" t="s">
+        <v>20</v>
+      </c>
+      <c r="I92" t="s">
+        <v>21</v>
+      </c>
+      <c r="J92" t="s">
+        <v>21</v>
+      </c>
+      <c r="K92" t="s">
+        <v>21</v>
+      </c>
+      <c r="L92" t="s">
+        <v>21</v>
+      </c>
+      <c r="M92" t="s">
+        <v>21</v>
+      </c>
+      <c r="N92" t="s">
+        <v>21</v>
+      </c>
+      <c r="O92" t="s">
+        <v>21</v>
+      </c>
+      <c r="P92" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
+      <c r="H99" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G103" s="4"/>
+      <c r="H103" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+      <c r="H113" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+      <c r="H115" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+      <c r="H117" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G119" s="4"/>
+      <c r="H119" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A87:G87"/>
+    <mergeCell ref="B87:G87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5824,24 +6904,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="12" width="14" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="16" width="18.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="17" max="19" width="24.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="20" max="22" width="16.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.42578125" style="8" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="255" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="16384" width="8.85546875" style="8" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="8" width="25.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="8" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="8" width="25.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="12.85546875" collapsed="true"/>
+    <col min="5" max="12" customWidth="true" style="8" width="14.0" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" style="8" width="18.42578125" collapsed="true"/>
+    <col min="17" max="19" customWidth="true" style="8" width="24.85546875" collapsed="true"/>
+    <col min="20" max="22" customWidth="true" style="8" width="16.28515625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="8" width="9.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="8" width="10.42578125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="8" width="62.0" collapsed="true"/>
+    <col min="26" max="16384" style="8" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -5989,7 +7069,7 @@
         <v>16</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>301</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -6661,4 +7741,199 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="255.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="R2" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="S2" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>358</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="M2" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>